<commit_message>
sqlite database and api to use it
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -20,18 +20,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">Column 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column 4</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+  <si>
+    <t xml:space="preserve">LSC Account Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area of Law</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjustment Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adjustment Reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount £</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0A123B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIVIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMRF Processing Delay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0B456C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urgent SMP adjustment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPOCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0C789D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDIATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly Payment</t>
   </si>
 </sst>
 </file>
@@ -41,11 +83,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -61,6 +104,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,7 +130,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -104,20 +154,33 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal 2" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -127,96 +190,96 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.53"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>20</v>
+      <c r="E4" s="2" t="n">
+        <v>300</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>